<commit_message>
Add changes for MODBUS documents
</commit_message>
<xml_diff>
--- a/Base/Base Changes Index.xlsx
+++ b/Base/Base Changes Index.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8848C58-EF24-48C8-84D8-933AE77552A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0BA038-792D-4030-865E-9425BF8EE954}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -555,6 +555,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1267,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1732,7 +1733,10 @@
       <c r="E24" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="4"/>
+      <c r="F24" s="16" t="str">
+        <f>HYPERLINK(".\Configure%20MODBUS%20TCP%20for%20Smart%20Meter.docx", "Configure ModBus TCP for Smart Meter")</f>
+        <v>Configure ModBus TCP for Smart Meter</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
@@ -1757,6 +1761,9 @@
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="12"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Finish Enhanced Logout Reminder Logic on Shift Change document
</commit_message>
<xml_diff>
--- a/Base/Base Changes Index.xlsx
+++ b/Base/Base Changes Index.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0BA038-792D-4030-865E-9425BF8EE954}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1902FBA-0611-45B6-ABC8-93E7F10C8BA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Changes</t>
   </si>
@@ -1270,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1451,7 +1451,10 @@
       <c r="E9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="16" t="str">
+        <f>HYPERLINK("./Synchronize%20Equipment%20Counter%20with%20Line%20During%20End%20Job.docx", "Synchronize Equipment Counter with Line During End Order")</f>
+        <v>Synchronize Equipment Counter with Line During End Order</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,7 +1530,9 @@
       <c r="E13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1602,8 +1607,8 @@
         <v>30</v>
       </c>
       <c r="F17" s="16" t="str">
-        <f>HYPERLINK("./Synchronize%20Equipment%20Counter%20with%20Line%20During%20End%20Job.docx", "Synchronize Equipment Counter with Line During End Order")</f>
-        <v>Synchronize Equipment Counter with Line During End Order</v>
+        <f>HYPERLINK("./Enhanced%20Logout%20Reminder%20Logic%20on%20Shift%20Change.docx", "Enhanced Logout Reminder Logic on Shift Change")</f>
+        <v>Enhanced Logout Reminder Logic on Shift Change</v>
       </c>
       <c r="G17" s="1"/>
     </row>

</xml_diff>

<commit_message>
Create Notification for EOHS Input Inspection document
</commit_message>
<xml_diff>
--- a/Base/Base Changes Index.xlsx
+++ b/Base/Base Changes Index.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDE51C3-1ABB-4401-B897-EE36570276E6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4450B3-3FEF-45E3-BE2B-782061163993}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>Changes</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>ngsfr_Intf_Item_Process_Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notification for EOHS Input during Combined Check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>operaDatalog_SX
+Script_Send_EOHS_Message</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1271,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F12" sqref="B12:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1747,12 +1756,25 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="4"/>
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="16" t="str">
+        <f>HYPERLINK(".\Notification%20for%20EOHS%20Input%20Inspection.docx", "Notification for EOHS Input Inspection")</f>
+        <v>Notification for EOHS Input Inspection</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>

</xml_diff>